<commit_message>
Added logs for dashcam test with noise tolerance set to 60, too high to be helpful
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\University\2019\Repositories\edgesum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B2ABF-5A50-4A04-B6C0-4CD249289EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFE2896-E163-45FB-B488-35E754D342E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{C9E8864D-5F17-466A-B1FF-8AA41EB8F054}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Size (MB)</t>
-  </si>
-  <si>
     <t>Length (s)</t>
   </si>
   <si>
@@ -84,18 +81,9 @@
     <t>Test game footage, 1920x1080 60FPS</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Summarisation time (s)</t>
   </si>
   <si>
-    <t>Summarised size (MB)</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t>1849s (30:49)</t>
   </si>
   <si>
-    <t>Actual total time:</t>
-  </si>
-  <si>
     <t>Actual total time</t>
   </si>
   <si>
@@ -139,6 +124,105 @@
   </si>
   <si>
     <t>1552s (25:52)</t>
+  </si>
+  <si>
+    <t>Summarised length (s)</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Dashcam footage, 1920x1080 60FPS</t>
+  </si>
+  <si>
+    <t>20191028_171616_NF</t>
+  </si>
+  <si>
+    <t>20191028_171716_NF</t>
+  </si>
+  <si>
+    <t>20191028_171746_EF</t>
+  </si>
+  <si>
+    <t>20191028_171846_NF</t>
+  </si>
+  <si>
+    <t>20191028_180605_NF</t>
+  </si>
+  <si>
+    <t>20191028_180615_EF</t>
+  </si>
+  <si>
+    <t>20191028_180715_NF</t>
+  </si>
+  <si>
+    <t>20191028_180815_NF</t>
+  </si>
+  <si>
+    <t>20191028_180915_NF</t>
+  </si>
+  <si>
+    <t>20191028_181015_NF</t>
+  </si>
+  <si>
+    <t>20191028_181115_NF</t>
+  </si>
+  <si>
+    <t>20191028_181159_PF</t>
+  </si>
+  <si>
+    <t>20191028_181359_PF</t>
+  </si>
+  <si>
+    <t>20191030_161051_NF</t>
+  </si>
+  <si>
+    <t>20191030_165129_NF</t>
+  </si>
+  <si>
+    <t>20191030_165229_NF</t>
+  </si>
+  <si>
+    <t>20191030_165329_NF</t>
+  </si>
+  <si>
+    <t>20191030_165429_NF</t>
+  </si>
+  <si>
+    <t>20191030_165530_NF</t>
+  </si>
+  <si>
+    <t>20191030_212910_NF</t>
+  </si>
+  <si>
+    <t>20191030_213010_NF</t>
+  </si>
+  <si>
+    <t>20191030_220901_NF</t>
+  </si>
+  <si>
+    <t>20191030_221001_NF</t>
+  </si>
+  <si>
+    <t>20191030_221101_NF</t>
+  </si>
+  <si>
+    <t>20191030_221201_NF</t>
+  </si>
+  <si>
+    <t>20191030_221302_NF</t>
+  </si>
+  <si>
+    <t>Size (KB)</t>
+  </si>
+  <si>
+    <t>Summarised size (KB)</t>
+  </si>
+  <si>
+    <t>829.817s (13:49.817)</t>
   </si>
 </sst>
 </file>
@@ -497,250 +581,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04285B5-A4B2-43D6-9C20-CE6D828CF8A2}">
-  <dimension ref="A2:E81"/>
+  <dimension ref="A2:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128:D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.06640625" customWidth="1"/>
     <col min="2" max="2" width="19.265625" customWidth="1"/>
     <col min="3" max="3" width="18.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
       <c r="B4">
-        <v>4.9800000000000004</v>
+        <v>5104</v>
       </c>
       <c r="C4">
-        <v>1.87</v>
+        <v>1916</v>
       </c>
       <c r="D4">
         <v>34</v>
       </c>
       <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>4.1399999999999997</v>
+        <v>4248</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>46</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>70.099999999999994</v>
+        <v>71856</v>
       </c>
       <c r="C6">
-        <v>70.099999999999994</v>
+        <v>71856</v>
       </c>
       <c r="D6">
         <v>59</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E6">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>17.8</v>
+        <v>18312</v>
       </c>
       <c r="C7">
-        <v>8.52</v>
+        <v>8728</v>
       </c>
       <c r="D7">
         <v>53</v>
       </c>
       <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>8.64</v>
+        <v>8856</v>
       </c>
       <c r="C8">
-        <v>3.9</v>
+        <v>3996</v>
       </c>
       <c r="D8">
         <v>30</v>
       </c>
       <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>12.3</v>
+        <v>12616</v>
       </c>
       <c r="C9">
-        <v>10.1</v>
+        <v>10376</v>
       </c>
       <c r="D9">
         <v>37</v>
       </c>
       <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>32.4</v>
+        <v>33220</v>
       </c>
       <c r="C10">
-        <v>17.100000000000001</v>
+        <v>17528</v>
       </c>
       <c r="D10">
         <v>55</v>
       </c>
       <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>45.2</v>
+        <v>46332</v>
       </c>
       <c r="C11">
-        <v>23.3</v>
+        <v>23924</v>
       </c>
       <c r="D11">
         <v>83</v>
       </c>
       <c r="E11">
+        <v>43</v>
+      </c>
+      <c r="F11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>15.2</v>
+        <v>15600</v>
       </c>
       <c r="C12">
-        <v>10.7</v>
+        <v>11040</v>
       </c>
       <c r="D12">
         <v>59</v>
       </c>
       <c r="E12">
+        <v>14</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>14.9</v>
+        <v>15272</v>
       </c>
       <c r="C13">
-        <v>10.5</v>
+        <v>10840</v>
       </c>
       <c r="D13">
         <v>61</v>
       </c>
       <c r="E13">
+        <v>14</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>15444</v>
       </c>
       <c r="C14">
-        <v>10.7</v>
+        <v>11028</v>
       </c>
       <c r="D14">
         <v>62</v>
       </c>
       <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>39.1</v>
+        <v>40128</v>
       </c>
       <c r="C15">
-        <v>37.9</v>
+        <v>38828</v>
       </c>
       <c r="D15">
         <v>62</v>
       </c>
       <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -748,12 +872,12 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>193</v>
@@ -761,7 +885,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>14</v>
@@ -769,7 +893,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>116</v>
@@ -777,7 +901,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22">
         <v>471</v>
@@ -785,7 +909,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>47</v>
@@ -793,7 +917,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>57</v>
@@ -801,7 +925,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>847</v>
@@ -809,7 +933,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>1212</v>
@@ -817,7 +941,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27">
         <v>91</v>
@@ -825,7 +949,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>91</v>
@@ -833,7 +957,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>93</v>
@@ -841,7 +965,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>109</v>
@@ -849,7 +973,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <f>SUM(B19:B30)</f>
@@ -858,20 +982,20 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -879,18 +1003,18 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>1.4</v>
@@ -904,7 +1028,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38">
         <v>13.7</v>
@@ -918,7 +1042,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>2.2000000000000002</v>
@@ -932,7 +1056,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40">
         <v>6.8</v>
@@ -946,7 +1070,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>3.5</v>
@@ -960,7 +1084,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -974,7 +1098,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B43">
         <f>SUM(B37:B42)</f>
@@ -991,7 +1115,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -999,24 +1123,24 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46">
         <v>0.8</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D46">
         <v>69</v>
@@ -1024,7 +1148,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47">
         <v>3.8</v>
@@ -1038,7 +1162,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48">
         <v>2.5</v>
@@ -1052,7 +1176,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
         <v>11.2</v>
@@ -1066,7 +1190,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50">
         <v>4.3</v>
@@ -1080,7 +1204,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>11.6</v>
@@ -1094,7 +1218,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B52">
         <f>SUM(B46:B51)</f>
@@ -1111,7 +1235,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B53">
         <f>SUM(B43,B52)</f>
@@ -1128,20 +1252,20 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
@@ -1149,18 +1273,18 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B59">
         <v>1.8</v>
@@ -1174,7 +1298,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B60">
         <v>4.2</v>
@@ -1188,7 +1312,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61">
         <v>5.5</v>
@@ -1202,7 +1326,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>3.7</v>
@@ -1216,7 +1340,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B63">
         <f>SUM(B59:B62)</f>
@@ -1233,7 +1357,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
@@ -1241,24 +1365,24 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D65" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66">
         <v>0.8</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D66">
         <v>36</v>
@@ -1266,7 +1390,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>2.1</v>
@@ -1280,7 +1404,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68">
         <v>14.9</v>
@@ -1294,7 +1418,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <v>3.5</v>
@@ -1308,7 +1432,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B70">
         <f>SUM(B66:B69)</f>
@@ -1325,7 +1449,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
@@ -1333,18 +1457,18 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D72" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73">
         <v>18.8</v>
@@ -1358,7 +1482,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74">
         <v>3.8</v>
@@ -1372,7 +1496,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75">
         <v>4.2</v>
@@ -1386,7 +1510,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B76">
         <v>12.1</v>
@@ -1400,7 +1524,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B77">
         <f>SUM(B73:B76)</f>
@@ -1417,7 +1541,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B78">
         <f>SUM(B63,B70,B77)</f>
@@ -1434,17 +1558,800 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" t="s">
+        <v>62</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>31</v>
+      </c>
+      <c r="F83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84">
+        <v>98500</v>
+      </c>
+      <c r="C84">
+        <v>98500</v>
+      </c>
+      <c r="D84">
+        <v>60</v>
+      </c>
+      <c r="E84">
+        <v>60</v>
+      </c>
+      <c r="F84" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85">
+        <v>57180</v>
+      </c>
+      <c r="C85">
+        <v>57180</v>
+      </c>
+      <c r="D85">
+        <v>35</v>
+      </c>
+      <c r="E85">
+        <v>35</v>
+      </c>
+      <c r="F85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86">
+        <v>98500</v>
+      </c>
+      <c r="C86">
+        <v>98500</v>
+      </c>
+      <c r="D86">
+        <v>60</v>
+      </c>
+      <c r="E86">
+        <v>60</v>
+      </c>
+      <c r="F86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87">
+        <v>98500</v>
+      </c>
+      <c r="C87">
+        <v>98500</v>
+      </c>
+      <c r="D87">
+        <v>60</v>
+      </c>
+      <c r="E87">
+        <v>60</v>
+      </c>
+      <c r="F87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88">
+        <v>24704</v>
+      </c>
+      <c r="C88">
+        <v>24704</v>
+      </c>
+      <c r="D88">
+        <v>14</v>
+      </c>
+      <c r="E88">
+        <v>14</v>
+      </c>
+      <c r="F88" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89">
+        <v>98500</v>
+      </c>
+      <c r="C89">
+        <v>89568</v>
+      </c>
+      <c r="D89">
+        <v>60</v>
+      </c>
+      <c r="E89">
+        <v>51</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90">
+        <v>98500</v>
+      </c>
+      <c r="C90">
+        <v>8872</v>
+      </c>
+      <c r="D90">
+        <v>60</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91">
+        <v>98500</v>
+      </c>
+      <c r="C91">
+        <v>3064</v>
+      </c>
+      <c r="D91">
+        <v>60</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92">
+        <v>98500</v>
+      </c>
+      <c r="C92">
+        <v>3068</v>
+      </c>
+      <c r="D92">
+        <v>60</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93">
+        <v>98500</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93">
+        <v>60</v>
+      </c>
+      <c r="E93" t="s">
+        <v>32</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94">
+        <v>78544</v>
+      </c>
+      <c r="C94" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94">
+        <v>48</v>
+      </c>
+      <c r="E94" t="s">
+        <v>32</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95">
+        <v>98500</v>
+      </c>
+      <c r="C95" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95">
+        <v>60</v>
+      </c>
+      <c r="E95" t="s">
+        <v>32</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96">
+        <v>98500</v>
+      </c>
+      <c r="C96" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96">
+        <v>60</v>
+      </c>
+      <c r="E96" t="s">
+        <v>32</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97">
+        <v>98500</v>
+      </c>
+      <c r="C97">
+        <v>58904</v>
+      </c>
+      <c r="D97">
+        <v>60</v>
+      </c>
+      <c r="E97">
+        <v>49</v>
+      </c>
+      <c r="F97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98">
+        <v>98500</v>
+      </c>
+      <c r="C98">
+        <v>13648</v>
+      </c>
+      <c r="D98">
+        <v>60</v>
+      </c>
+      <c r="E98">
+        <v>21</v>
+      </c>
+      <c r="F98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99">
+        <v>98500</v>
+      </c>
+      <c r="C99" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99">
+        <v>60</v>
+      </c>
+      <c r="E99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>51</v>
+      </c>
+      <c r="B100">
+        <v>98500</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100">
+        <v>60</v>
+      </c>
+      <c r="E100" t="s">
+        <v>32</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>52</v>
+      </c>
+      <c r="B101">
+        <v>98500</v>
+      </c>
+      <c r="C101">
+        <v>6540</v>
+      </c>
+      <c r="D101">
+        <v>60</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102">
+        <v>31328</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102">
+        <v>19</v>
+      </c>
+      <c r="E102" t="s">
+        <v>32</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103">
+        <v>98500</v>
+      </c>
+      <c r="C103" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103">
+        <v>60</v>
+      </c>
+      <c r="E103" t="s">
+        <v>32</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104">
+        <v>98500</v>
+      </c>
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104">
+        <v>60</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>56</v>
+      </c>
+      <c r="B105">
+        <v>98500</v>
+      </c>
+      <c r="C105">
+        <v>55400</v>
+      </c>
+      <c r="D105">
+        <v>60</v>
+      </c>
+      <c r="E105">
+        <v>36</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>57</v>
+      </c>
+      <c r="B106">
+        <v>98500</v>
+      </c>
+      <c r="C106">
+        <v>23396</v>
+      </c>
+      <c r="D106">
+        <v>60</v>
+      </c>
+      <c r="E106">
+        <v>28</v>
+      </c>
+      <c r="F106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>58</v>
+      </c>
+      <c r="B107">
+        <v>98500</v>
+      </c>
+      <c r="C107" t="s">
+        <v>32</v>
+      </c>
+      <c r="D107">
+        <v>60</v>
+      </c>
+      <c r="E107" t="s">
+        <v>32</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>59</v>
+      </c>
+      <c r="B108">
+        <v>98500</v>
+      </c>
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108">
+        <v>60</v>
+      </c>
+      <c r="E108" t="s">
+        <v>32</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>60</v>
+      </c>
+      <c r="B109">
+        <v>98500</v>
+      </c>
+      <c r="C109">
+        <v>24308</v>
+      </c>
+      <c r="D109">
+        <v>60</v>
+      </c>
+      <c r="E109">
+        <v>30</v>
+      </c>
+      <c r="F109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>35</v>
+      </c>
+      <c r="B113">
+        <v>26.439</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>36</v>
+      </c>
+      <c r="B114">
+        <v>15.901</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115">
+        <v>26.736999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>38</v>
+      </c>
+      <c r="B116">
+        <v>27.82</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>39</v>
+      </c>
+      <c r="B117">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>40</v>
+      </c>
+      <c r="B118">
+        <v>30.199000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B119">
+        <v>36.860999999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>42</v>
+      </c>
+      <c r="B120">
+        <v>36.716000000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>43</v>
+      </c>
+      <c r="B121">
+        <v>36.561999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>44</v>
+      </c>
+      <c r="B122">
+        <v>35.945999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>45</v>
+      </c>
+      <c r="B123">
+        <v>26.963999999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>46</v>
+      </c>
+      <c r="B124">
+        <v>36.438000000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>47</v>
+      </c>
+      <c r="B125">
+        <v>36.392000000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>48</v>
+      </c>
+      <c r="B126">
+        <v>35.395000000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>49</v>
+      </c>
+      <c r="B127">
+        <v>36.844999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>50</v>
+      </c>
+      <c r="B128">
+        <v>36.81</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>51</v>
+      </c>
+      <c r="B129">
+        <v>36.780999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>52</v>
+      </c>
+      <c r="B130">
+        <v>35.555999999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>53</v>
+      </c>
+      <c r="B131">
+        <v>11.531000000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132">
+        <v>37.35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>55</v>
+      </c>
+      <c r="B133">
+        <v>37.948999999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>56</v>
+      </c>
+      <c r="B134">
+        <v>35.667000000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>57</v>
+      </c>
+      <c r="B135">
+        <v>35.738999999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>58</v>
+      </c>
+      <c r="B136">
+        <v>37.073999999999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>59</v>
+      </c>
+      <c r="B137">
+        <v>36.835000000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>60</v>
+      </c>
+      <c r="B138">
+        <v>36.14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>17</v>
+      </c>
+      <c r="B139">
+        <f>SUM(B113:B138)</f>
+        <v>829.81700000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>27</v>
+      </c>
+      <c r="B140" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added logs for dashcam test with noise tolerance set to 38
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\University\2019\Repositories\edgesum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFE2896-E163-45FB-B488-35E754D342E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458C791-96FC-4C5C-9BD8-A10DE21D3694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{C9E8864D-5F17-466A-B1FF-8AA41EB8F054}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Offline (s8)</t>
-  </si>
-  <si>
     <t>Three nodes (n5x-34d8 master)</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>Dashcam footage, 1920x1080 60FPS</t>
-  </si>
-  <si>
     <t>20191028_171616_NF</t>
   </si>
   <si>
@@ -222,13 +216,31 @@
     <t>Summarised size (KB)</t>
   </si>
   <si>
-    <t>829.817s (13:49.817)</t>
+    <t>1890.938s (31:30.938)</t>
+  </si>
+  <si>
+    <t>Dashcam footage, 1920x1080 60FPS, 38 noise tolerance</t>
+  </si>
+  <si>
+    <t>2815.272s (46:55.272)</t>
+  </si>
+  <si>
+    <t>Offline - s8</t>
+  </si>
+  <si>
+    <t>Offline - n5</t>
+  </si>
+  <si>
+    <t>6591.254s (1:49:51.254)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,9 +276,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04285B5-A4B2-43D6-9C20-CE6D828CF8A2}">
-  <dimension ref="A2:F140"/>
+  <dimension ref="A2:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128:D129"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -607,16 +620,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -630,13 +643,13 @@
         <v>5104</v>
       </c>
       <c r="C4">
-        <v>1916</v>
+        <v>1724</v>
       </c>
       <c r="D4">
         <v>34</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -650,13 +663,13 @@
         <v>4248</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -679,7 +692,7 @@
         <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -710,16 +723,16 @@
         <v>8856</v>
       </c>
       <c r="C8">
-        <v>3996</v>
+        <v>6932</v>
       </c>
       <c r="D8">
         <v>30</v>
       </c>
       <c r="E8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -750,16 +763,16 @@
         <v>33220</v>
       </c>
       <c r="C10">
-        <v>17528</v>
+        <v>17308</v>
       </c>
       <c r="D10">
         <v>55</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -770,13 +783,13 @@
         <v>46332</v>
       </c>
       <c r="C11">
-        <v>23924</v>
+        <v>23704</v>
       </c>
       <c r="D11">
         <v>83</v>
       </c>
       <c r="E11">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -830,13 +843,13 @@
         <v>15444</v>
       </c>
       <c r="C14">
-        <v>11028</v>
+        <v>10648</v>
       </c>
       <c r="D14">
         <v>62</v>
       </c>
       <c r="E14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -864,7 +877,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -982,20 +995,20 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
         <v>27</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -1003,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
@@ -1115,7 +1128,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -1123,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
@@ -1140,7 +1153,7 @@
         <v>0.8</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46">
         <v>69</v>
@@ -1235,7 +1248,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B53">
         <f>SUM(B43,B52)</f>
@@ -1252,20 +1265,20 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
@@ -1273,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
@@ -1357,7 +1370,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
@@ -1365,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D65" t="s">
         <v>16</v>
@@ -1382,7 +1395,7 @@
         <v>0.8</v>
       </c>
       <c r="C66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D66">
         <v>36</v>
@@ -1449,7 +1462,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
@@ -1457,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
         <v>16</v>
@@ -1541,7 +1554,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B78">
         <f>SUM(B63,B70,B77)</f>
@@ -1558,10 +1571,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
@@ -1572,7 +1585,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
@@ -1580,16 +1593,16 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F83" t="s">
         <v>2</v>
@@ -1597,7 +1610,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B84">
         <v>98500</v>
@@ -1612,12 +1625,12 @@
         <v>60</v>
       </c>
       <c r="F84" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B85">
         <v>57180</v>
@@ -1632,12 +1645,12 @@
         <v>35</v>
       </c>
       <c r="F85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B86">
         <v>98500</v>
@@ -1652,12 +1665,12 @@
         <v>60</v>
       </c>
       <c r="F86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B87">
         <v>98500</v>
@@ -1672,12 +1685,12 @@
         <v>60</v>
       </c>
       <c r="F87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B88">
         <v>24704</v>
@@ -1692,104 +1705,104 @@
         <v>14</v>
       </c>
       <c r="F88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B89">
         <v>98500</v>
       </c>
       <c r="C89">
-        <v>89568</v>
+        <v>86020</v>
       </c>
       <c r="D89">
         <v>60</v>
       </c>
       <c r="E89">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F89">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B90">
         <v>98500</v>
       </c>
       <c r="C90">
-        <v>8872</v>
+        <v>14712</v>
       </c>
       <c r="D90">
         <v>60</v>
       </c>
       <c r="E90">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B91">
         <v>98500</v>
       </c>
-      <c r="C91">
-        <v>3064</v>
+      <c r="C91" t="s">
+        <v>31</v>
       </c>
       <c r="D91">
         <v>60</v>
       </c>
-      <c r="E91">
-        <v>2</v>
+      <c r="E91" t="s">
+        <v>31</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B92">
         <v>98500</v>
       </c>
-      <c r="C92">
-        <v>3068</v>
+      <c r="C92" t="s">
+        <v>31</v>
       </c>
       <c r="D92">
         <v>60</v>
       </c>
-      <c r="E92">
-        <v>1</v>
+      <c r="E92" t="s">
+        <v>31</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B93">
         <v>98500</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D93">
         <v>60</v>
       </c>
       <c r="E93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -1797,19 +1810,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B94">
         <v>78544</v>
       </c>
       <c r="C94" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D94">
         <v>48</v>
       </c>
       <c r="E94" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -1817,19 +1830,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B95">
         <v>98500</v>
       </c>
       <c r="C95" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D95">
         <v>60</v>
       </c>
       <c r="E95" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -1837,19 +1850,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B96">
         <v>98500</v>
       </c>
       <c r="C96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D96">
         <v>60</v>
       </c>
       <c r="E96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -1857,39 +1870,39 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B97">
         <v>98500</v>
       </c>
       <c r="C97">
-        <v>58904</v>
+        <v>41600</v>
       </c>
       <c r="D97">
         <v>60</v>
       </c>
       <c r="E97">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F97">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B98">
         <v>98500</v>
       </c>
       <c r="C98">
-        <v>13648</v>
+        <v>8904</v>
       </c>
       <c r="D98">
         <v>60</v>
       </c>
       <c r="E98">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F98">
         <v>2</v>
@@ -1897,19 +1910,19 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B99">
         <v>98500</v>
       </c>
       <c r="C99" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D99">
         <v>60</v>
       </c>
       <c r="E99" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -1917,19 +1930,19 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B100">
         <v>98500</v>
       </c>
       <c r="C100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D100">
         <v>60</v>
       </c>
       <c r="E100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -1937,7 +1950,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B101">
         <v>98500</v>
@@ -1957,19 +1970,19 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B102">
         <v>31328</v>
       </c>
       <c r="C102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D102">
         <v>19</v>
       </c>
       <c r="E102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -1977,19 +1990,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B103">
         <v>98500</v>
       </c>
       <c r="C103" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D103">
         <v>60</v>
       </c>
       <c r="E103" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -1997,19 +2010,19 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B104">
         <v>98500</v>
       </c>
       <c r="C104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D104">
         <v>60</v>
       </c>
       <c r="E104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -2017,7 +2030,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B105">
         <v>98500</v>
@@ -2037,39 +2050,39 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B106">
         <v>98500</v>
       </c>
       <c r="C106">
-        <v>23396</v>
+        <v>22000</v>
       </c>
       <c r="D106">
         <v>60</v>
       </c>
       <c r="E106">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B107">
         <v>98500</v>
       </c>
       <c r="C107" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D107">
         <v>60</v>
       </c>
       <c r="E107" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -2077,19 +2090,19 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B108">
         <v>98500</v>
       </c>
       <c r="C108" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D108">
         <v>60</v>
       </c>
       <c r="E108" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -2097,13 +2110,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B109">
         <v>98500</v>
       </c>
       <c r="C109">
-        <v>24308</v>
+        <v>24356</v>
       </c>
       <c r="D109">
         <v>60</v>
@@ -2117,7 +2130,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
@@ -2130,210 +2143,210 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>35</v>
-      </c>
-      <c r="B113">
-        <v>26.439</v>
+        <v>33</v>
+      </c>
+      <c r="B113" s="2">
+        <v>32.411999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>36</v>
-      </c>
-      <c r="B114">
-        <v>15.901</v>
+        <v>34</v>
+      </c>
+      <c r="B114" s="2">
+        <v>16.224</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>37</v>
-      </c>
-      <c r="B115">
-        <v>26.736999999999998</v>
+        <v>35</v>
+      </c>
+      <c r="B115" s="2">
+        <v>29.66</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>38</v>
-      </c>
-      <c r="B116">
-        <v>27.82</v>
+        <v>36</v>
+      </c>
+      <c r="B116" s="2">
+        <v>33.314</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>39</v>
-      </c>
-      <c r="B117">
-        <v>7.17</v>
+        <v>37</v>
+      </c>
+      <c r="B117" s="2">
+        <v>8.7129999999999992</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>40</v>
-      </c>
-      <c r="B118">
-        <v>30.199000000000002</v>
+        <v>38</v>
+      </c>
+      <c r="B118" s="2">
+        <v>382.50599999999997</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>41</v>
-      </c>
-      <c r="B119">
-        <v>36.860999999999997</v>
+        <v>39</v>
+      </c>
+      <c r="B119" s="2">
+        <v>33.476999999999997</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>42</v>
-      </c>
-      <c r="B120">
-        <v>36.716000000000001</v>
+        <v>40</v>
+      </c>
+      <c r="B120" s="2">
+        <v>33.414000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>43</v>
-      </c>
-      <c r="B121">
-        <v>36.561999999999998</v>
+        <v>41</v>
+      </c>
+      <c r="B121" s="2">
+        <v>33.99</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>44</v>
-      </c>
-      <c r="B122">
-        <v>35.945999999999998</v>
+        <v>42</v>
+      </c>
+      <c r="B122" s="2">
+        <v>32.436999999999998</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>45</v>
-      </c>
-      <c r="B123">
-        <v>26.963999999999999</v>
+        <v>43</v>
+      </c>
+      <c r="B123" s="2">
+        <v>24.617000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>46</v>
-      </c>
-      <c r="B124">
-        <v>36.438000000000002</v>
+        <v>44</v>
+      </c>
+      <c r="B124" s="2">
+        <v>33.883000000000003</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>47</v>
-      </c>
-      <c r="B125">
-        <v>36.392000000000003</v>
+        <v>45</v>
+      </c>
+      <c r="B125" s="2">
+        <v>33.465000000000003</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>48</v>
-      </c>
-      <c r="B126">
-        <v>35.395000000000003</v>
+        <v>46</v>
+      </c>
+      <c r="B126" s="2">
+        <v>185.27500000000001</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>49</v>
-      </c>
-      <c r="B127">
-        <v>36.844999999999999</v>
+        <v>47</v>
+      </c>
+      <c r="B127" s="2">
+        <v>121.431</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>50</v>
-      </c>
-      <c r="B128">
-        <v>36.81</v>
+        <v>48</v>
+      </c>
+      <c r="B128" s="2">
+        <v>34.451999999999998</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>51</v>
-      </c>
-      <c r="B129">
-        <v>36.780999999999999</v>
+        <v>49</v>
+      </c>
+      <c r="B129" s="2">
+        <v>34.03</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>52</v>
-      </c>
-      <c r="B130">
-        <v>35.555999999999997</v>
+        <v>50</v>
+      </c>
+      <c r="B130" s="2">
+        <v>31.443999999999999</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>53</v>
-      </c>
-      <c r="B131">
-        <v>11.531000000000001</v>
+        <v>51</v>
+      </c>
+      <c r="B131" s="2">
+        <v>11.074</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>54</v>
-      </c>
-      <c r="B132">
-        <v>37.35</v>
+        <v>52</v>
+      </c>
+      <c r="B132" s="2">
+        <v>34.514000000000003</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>55</v>
-      </c>
-      <c r="B133">
-        <v>37.948999999999998</v>
+        <v>53</v>
+      </c>
+      <c r="B133" s="2">
+        <v>34.106000000000002</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>56</v>
-      </c>
-      <c r="B134">
-        <v>35.667000000000002</v>
+        <v>54</v>
+      </c>
+      <c r="B134" s="2">
+        <v>34.918999999999997</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>57</v>
-      </c>
-      <c r="B135">
-        <v>35.738999999999997</v>
+        <v>55</v>
+      </c>
+      <c r="B135" s="2">
+        <v>252.988</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>58</v>
-      </c>
-      <c r="B136">
-        <v>37.073999999999998</v>
+        <v>56</v>
+      </c>
+      <c r="B136" s="2">
+        <v>38.369999999999997</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>59</v>
-      </c>
-      <c r="B137">
-        <v>36.835000000000001</v>
+        <v>57</v>
+      </c>
+      <c r="B137" s="2">
+        <v>39.002000000000002</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>60</v>
-      </c>
-      <c r="B138">
-        <v>36.14</v>
+        <v>58</v>
+      </c>
+      <c r="B138" s="2">
+        <v>311.221</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
@@ -2342,14 +2355,754 @@
       </c>
       <c r="B139">
         <f>SUM(B113:B138)</f>
-        <v>829.81700000000001</v>
+        <v>1890.9379999999999</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B140" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>33</v>
+      </c>
+      <c r="B144" s="2">
+        <v>114.48</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>34</v>
+      </c>
+      <c r="B145" s="2">
+        <v>60.122</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>35</v>
+      </c>
+      <c r="B146" s="2">
+        <v>117.824</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>36</v>
+      </c>
+      <c r="B147" s="2">
+        <v>112.123</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148" s="2">
+        <v>30.231999999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>38</v>
+      </c>
+      <c r="B149" s="2">
+        <v>1218.2929999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>39</v>
+      </c>
+      <c r="B150" s="2">
+        <v>134.45099999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>40</v>
+      </c>
+      <c r="B151" s="2">
+        <v>114.49</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>41</v>
+      </c>
+      <c r="B152" s="2">
+        <v>134.398</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>42</v>
+      </c>
+      <c r="B153" s="2">
+        <v>112.825</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>43</v>
+      </c>
+      <c r="B154" s="2">
+        <v>84.173000000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>44</v>
+      </c>
+      <c r="B155" s="2">
+        <v>132.29599999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>45</v>
+      </c>
+      <c r="B156" s="2">
+        <v>132.77000000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>46</v>
+      </c>
+      <c r="B157" s="2">
+        <v>738.52499999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>47</v>
+      </c>
+      <c r="B158" s="2">
+        <v>516.70699999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>48</v>
+      </c>
+      <c r="B159" s="2">
+        <v>147.51300000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A160" t="s">
+        <v>49</v>
+      </c>
+      <c r="B160" s="2">
+        <v>146.33199999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>50</v>
+      </c>
+      <c r="B161" s="2">
+        <v>259.10199999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>51</v>
+      </c>
+      <c r="B162" s="2">
+        <v>41.496000000000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>52</v>
+      </c>
+      <c r="B163" s="2">
+        <v>143.52000000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>53</v>
+      </c>
+      <c r="B164" s="2">
+        <v>112.99299999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>54</v>
+      </c>
+      <c r="B165" s="2">
+        <v>110.06</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>55</v>
+      </c>
+      <c r="B166" s="2">
+        <v>749.572</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A167" t="s">
+        <v>56</v>
+      </c>
+      <c r="B167" s="2">
+        <v>143.71700000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>57</v>
+      </c>
+      <c r="B168" s="2">
+        <v>143.56399999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A169" t="s">
+        <v>58</v>
+      </c>
+      <c r="B169" s="2">
+        <v>839.67600000000004</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A170" t="s">
+        <v>17</v>
+      </c>
+      <c r="B170" s="2">
+        <f>SUM(B144:B169)</f>
+        <v>6591.2540000000017</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A171" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A173" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" t="s">
+        <v>20</v>
+      </c>
+      <c r="C175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A176" t="s">
+        <v>33</v>
+      </c>
+      <c r="B176" s="2">
+        <v>13.904</v>
+      </c>
+      <c r="C176" s="2">
+        <v>43.66</v>
+      </c>
+      <c r="D176" s="2">
+        <v>76.697000000000003</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A177" t="s">
+        <v>36</v>
+      </c>
+      <c r="B177" s="2">
+        <v>28.797000000000001</v>
+      </c>
+      <c r="C177" s="2">
+        <v>40.194000000000003</v>
+      </c>
+      <c r="D177" s="2">
+        <v>121.095</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A178" t="s">
+        <v>39</v>
+      </c>
+      <c r="B178" s="2">
+        <v>89.198999999999998</v>
+      </c>
+      <c r="C178" s="2">
+        <v>12.573</v>
+      </c>
+      <c r="D178" s="2">
+        <v>111.64700000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A179" t="s">
+        <v>42</v>
+      </c>
+      <c r="B179" s="2">
+        <v>171.70699999999999</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D179" s="2">
+        <v>109.09</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A180" t="s">
+        <v>45</v>
+      </c>
+      <c r="B180" s="2">
+        <v>170.92500000000001</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D180" s="2">
+        <v>109.452</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A181" t="s">
+        <v>48</v>
+      </c>
+      <c r="B181" s="2">
+        <v>200.339</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D181" s="2">
+        <v>111.417</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A182" t="s">
+        <v>51</v>
+      </c>
+      <c r="B182" s="2">
+        <v>216.51499999999999</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D182" s="2">
+        <v>38.741999999999997</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A183" t="s">
+        <v>54</v>
+      </c>
+      <c r="B183" s="2">
+        <v>205.79599999999999</v>
+      </c>
+      <c r="C183" s="2">
+        <v>46.170999999999999</v>
+      </c>
+      <c r="D183" s="2">
+        <v>112.41200000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A184" t="s">
+        <v>57</v>
+      </c>
+      <c r="B184" s="2">
+        <v>222.82900000000001</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D184" s="2">
+        <v>113.931</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A185" t="s">
+        <v>17</v>
+      </c>
+      <c r="B185" s="2">
+        <f>SUM(B176:B184)</f>
+        <v>1320.011</v>
+      </c>
+      <c r="C185" s="2">
+        <f>SUM(C176:C184)</f>
+        <v>142.59799999999998</v>
+      </c>
+      <c r="D185" s="2">
+        <f>SUM(D176:D184)</f>
+        <v>904.48300000000006</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A186" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A187" t="s">
+        <v>0</v>
+      </c>
+      <c r="B187" t="s">
+        <v>20</v>
+      </c>
+      <c r="C187" t="s">
+        <v>28</v>
+      </c>
+      <c r="D187" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A188" t="s">
+        <v>34</v>
+      </c>
+      <c r="B188" s="2">
+        <v>13.872999999999999</v>
+      </c>
+      <c r="C188" s="2">
+        <v>37.994999999999997</v>
+      </c>
+      <c r="D188" s="2">
+        <v>36.906999999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A189" t="s">
+        <v>37</v>
+      </c>
+      <c r="B189" s="2">
+        <v>27.702999999999999</v>
+      </c>
+      <c r="C189" s="2">
+        <v>23.370999999999999</v>
+      </c>
+      <c r="D189" s="2">
+        <v>19.207999999999998</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A190" t="s">
+        <v>40</v>
+      </c>
+      <c r="B190" s="2">
+        <v>119.154</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D190" s="2">
+        <v>67.617999999999995</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A191" t="s">
+        <v>43</v>
+      </c>
+      <c r="B191" s="2">
+        <v>150.96199999999999</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D191" s="2">
+        <v>54.457999999999998</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A192" t="s">
+        <v>46</v>
+      </c>
+      <c r="B192" s="2">
+        <v>194.553</v>
+      </c>
+      <c r="C192" s="2">
+        <v>19.652999999999999</v>
+      </c>
+      <c r="D192" s="2">
+        <v>625.08500000000004</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A193" t="s">
+        <v>49</v>
+      </c>
+      <c r="B193" s="2">
+        <v>216.32499999999999</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D193" s="2">
+        <v>110.077</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A194" t="s">
+        <v>52</v>
+      </c>
+      <c r="B194" s="2">
+        <v>198.797</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D194" s="2">
+        <v>111.988</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A195" t="s">
+        <v>55</v>
+      </c>
+      <c r="B195" s="2">
+        <v>194.25899999999999</v>
+      </c>
+      <c r="C195" s="2">
+        <v>10.496</v>
+      </c>
+      <c r="D195" s="2">
+        <v>711.27300000000002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A196" t="s">
+        <v>58</v>
+      </c>
+      <c r="B196" s="2">
+        <v>235.27500000000001</v>
+      </c>
+      <c r="C196" s="2">
+        <v>8.6170000000000009</v>
+      </c>
+      <c r="D196" s="2">
+        <v>792.52300000000002</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A197" t="s">
+        <v>17</v>
+      </c>
+      <c r="B197" s="2">
+        <f>SUM(B188:B196)</f>
+        <v>1350.9010000000001</v>
+      </c>
+      <c r="C197" s="2">
+        <f>SUM(C188:C196)</f>
+        <v>100.13200000000001</v>
+      </c>
+      <c r="D197" s="2">
+        <f>SUM(D188:D196)</f>
+        <v>2529.1370000000002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A199" t="s">
+        <v>0</v>
+      </c>
+      <c r="B199" t="s">
+        <v>20</v>
+      </c>
+      <c r="C199" t="s">
+        <v>28</v>
+      </c>
+      <c r="D199" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A200" t="s">
+        <v>35</v>
+      </c>
+      <c r="B200" s="2">
+        <v>24.14</v>
+      </c>
+      <c r="C200" s="2">
+        <v>59.478999999999999</v>
+      </c>
+      <c r="D200" s="2">
+        <v>124.32</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A201" t="s">
+        <v>38</v>
+      </c>
+      <c r="B201" s="2">
+        <v>39.274000000000001</v>
+      </c>
+      <c r="C201" s="2">
+        <v>42.43</v>
+      </c>
+      <c r="D201" s="2">
+        <v>1269.1590000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A202" t="s">
+        <v>41</v>
+      </c>
+      <c r="B202" s="2">
+        <v>152.30799999999999</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D202" s="2">
+        <v>109.407</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A203" t="s">
+        <v>44</v>
+      </c>
+      <c r="B203" s="2">
+        <v>144.917</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D203" s="2">
+        <v>134.42599999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A204" t="s">
+        <v>47</v>
+      </c>
+      <c r="B204" s="2">
+        <v>191.40600000000001</v>
+      </c>
+      <c r="C204" s="2">
+        <v>6.4820000000000002</v>
+      </c>
+      <c r="D204" s="2">
+        <v>393.61799999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A205" t="s">
+        <v>50</v>
+      </c>
+      <c r="B205" s="2">
+        <v>237.52099999999999</v>
+      </c>
+      <c r="C205" s="2">
+        <v>3.2639999999999998</v>
+      </c>
+      <c r="D205" s="2">
+        <v>100.39</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>53</v>
+      </c>
+      <c r="B206" s="2">
+        <v>210.92400000000001</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D206" s="2">
+        <v>110.233</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A207" t="s">
+        <v>56</v>
+      </c>
+      <c r="B207" s="2">
+        <v>208.125</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D207" s="2">
+        <v>114.337</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A208" t="s">
+        <v>17</v>
+      </c>
+      <c r="B208" s="2">
+        <f>SUM(B200:B207)</f>
+        <v>1208.615</v>
+      </c>
+      <c r="C208" s="2">
+        <f>SUM(C200:C207)</f>
+        <v>111.65499999999999</v>
+      </c>
+      <c r="D208" s="2">
+        <f>SUM(D200:D207)</f>
+        <v>2355.89</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A209" t="s">
+        <v>22</v>
+      </c>
+      <c r="B209" s="2">
+        <f>SUM(B185,B197,B208)</f>
+        <v>3879.527</v>
+      </c>
+      <c r="C209" s="2">
+        <f>SUM(C185,C197,C208)</f>
+        <v>354.38499999999999</v>
+      </c>
+      <c r="D209" s="2">
+        <f>SUM(D185,D197,D208)</f>
+        <v>5789.51</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A210" t="s">
+        <v>26</v>
+      </c>
+      <c r="B210" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started work on some graphs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\University\2019\Repositories\edgesum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458C791-96FC-4C5C-9BD8-A10DE21D3694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4252C2-9061-4564-88CD-3655EBF84131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{C9E8864D-5F17-466A-B1FF-8AA41EB8F054}"/>
   </bookViews>
@@ -297,6 +297,4914 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size (KB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>test07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>test09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>test10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>test11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71856</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12616</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46332</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15272</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15444</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A962-47D8-BC08-55E2170394FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Summarised size (KB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1724</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71856</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6932</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10376</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11040</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10840</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10648</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38828</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A962-47D8-BC08-55E2170394FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="503802480"/>
+        <c:axId val="503802808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="503802480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503802808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="503802808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503802480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Length (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>test07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>test09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>test10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>test11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2D7-49AD-B290-1DF423D959ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Summarised length (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>test07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>test09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>test10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>test11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A2D7-49AD-B290-1DF423D959ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="594033360"/>
+        <c:axId val="594034344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="594033360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594034344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594034344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594033360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$17:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Offline - s8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Summarisation time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>test07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>test09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>test10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>test11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6AA-4D03-9BE0-A0845AE4E865}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="503802152"/>
+        <c:axId val="503799200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="503802152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503799200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="503799200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503802152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>n5x-9c8f Transfer Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Transfer time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$37:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3818-4040-A590-A5C6ED173703}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Return time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$37:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$37:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3818-4040-A590-A5C6ED173703}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="665658800"/>
+        <c:axId val="665661752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="665658800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665661752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665661752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665658800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>n5x-9c8f Summarisation Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Summarisation time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$37:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>test00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>test04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>test06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>test08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>test10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$37:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75E3-4B59-97A9-FBA8CE1D29C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="654079376"/>
+        <c:axId val="654089544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="654079376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654089544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="654089544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654079376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>235743</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>111918</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D324EE-3638-4CCF-8386-A0D080FC4680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>316706</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>78580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2278FAC9-ED09-487B-9345-50A4FC703A92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>812005</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>40481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>521492</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>69056</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F698C348-F618-43B7-AE1C-368CE91A388C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>97631</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>173830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>535781</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>21430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBA80511-E4E5-4AE0-A9CF-127827F1C94F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>628649</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEA9EC75-C898-40CC-BDBE-51D1C1D216F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -596,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04285B5-A4B2-43D6-9C20-CE6D828CF8A2}">
   <dimension ref="A2:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" activeCellId="1" sqref="A36:A42 D36:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3110,5 +8018,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>